<commit_message>
SCD0314, SCD0315, SCD0316, SCD0317
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0314 - Pimpinan Cabang dan Penyelia SRM Melakukan cancel pengajuan di setujui.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0314 - Pimpinan Cabang dan Penyelia SRM Melakukan cancel pengajuan di setujui.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5BE7BB-B8D4-4342-A1BE-6E3B4ACEE3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C9AFC5-1411-4E19-89E4-9578EEA2B355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0314" sheetId="2" r:id="rId1"/>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,11 +652,11 @@
       </c>
       <c r="M2" s="13" t="str">
         <f ca="1">TEXT(TODAY(),"yyyy-mm-dd")</f>
-        <v>2022-09-05</v>
+        <v>2022-09-06</v>
       </c>
       <c r="N2" s="13" t="str">
         <f ca="1">TEXT(TODAY()+30,"yyyy-mm-dd")</f>
-        <v>2022-10-05</v>
+        <v>2022-10-06</v>
       </c>
       <c r="O2" s="14" t="s">
         <v>21</v>
@@ -739,11 +739,11 @@
       </c>
       <c r="M4" s="13" t="str">
         <f ca="1">TEXT(TODAY(),"yyyy-mm-dd")</f>
-        <v>2022-09-05</v>
+        <v>2022-09-06</v>
       </c>
       <c r="N4" s="13" t="str">
         <f ca="1">TEXT(TODAY()+30,"yyyy-mm-dd")</f>
-        <v>2022-10-05</v>
+        <v>2022-10-06</v>
       </c>
       <c r="O4" s="14" t="s">
         <v>21</v>

</xml_diff>